<commit_message>
add anotation and modify config file
</commit_message>
<xml_diff>
--- a/Calculate-Total-Cost-Dispatcher/Data/Config.xlsx
+++ b/Calculate-Total-Cost-Dispatcher/Data/Config.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P15\Documents\UiPath\Calculate-Total-Cost\Calculate-Total-Cost-Dispatcher\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879B0038-D53F-4B10-8809-F5CA3F945528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9707"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -70,27 +76,18 @@
     <t>InputFolderPath</t>
   </si>
   <si>
-    <t>Calculate-Total-Cost-Dispatcher\Data\Input\</t>
-  </si>
-  <si>
     <t>Path to Input folder contains data for dispatcher process</t>
   </si>
   <si>
     <t>SuccessFolderPath</t>
   </si>
   <si>
-    <t>Calculate-Total-Cost-Dispatcher\Data\Success\</t>
-  </si>
-  <si>
     <t>Path to Input folder contains success data for dispatcher process</t>
   </si>
   <si>
     <t>FailedFolderPath</t>
   </si>
   <si>
-    <t>Calculate-Total-Cost-Dispatcher\Data\Failed\</t>
-  </si>
-  <si>
     <t>Path to Input folder contains failed data for dispatcher process</t>
   </si>
   <si>
@@ -203,19 +200,22 @@
   </si>
   <si>
     <t>Description (Assets will always overwrite other config)</t>
+  </si>
+  <si>
+    <t>Data\Input\</t>
+  </si>
+  <si>
+    <t>Data\Success\</t>
+  </si>
+  <si>
+    <t>Data\Failed\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -242,345 +242,16 @@
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -588,249 +259,10 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -842,63 +274,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1156,27 +545,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4444444444444" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5555555555556" customWidth="1"/>
-    <col min="2" max="2" width="69.2222222222222" customWidth="1"/>
-    <col min="3" max="3" width="81.4444444444444" customWidth="1"/>
-    <col min="4" max="26" width="8.66666666666667" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="2" max="2" width="69.21875" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1" spans="1:26">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1210,7 +599,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1" spans="1:3">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1221,7 +610,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" ht="43.2" spans="1:3">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1232,7 +621,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" ht="28.8" spans="1:3">
+    <row r="4" spans="1:26" ht="28.8">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1243,58 +632,58 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1" spans="1:3">
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="s">
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1" spans="1:3">
-      <c r="A6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1" spans="1:3">
-      <c r="A7" s="3" t="s">
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1" spans="1:3">
-      <c r="A8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" ht="14.25" customHeight="1"/>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -2278,32 +1667,30 @@
     <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" display="https://drive.google.com/drive/folders/1GQbDKmV-dNwHf9gkuJXI6AP49jhCwram"/>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4444444444444" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.4444444444444" customWidth="1"/>
-    <col min="4" max="26" width="8.66666666666667" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1" spans="1:26">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2337,157 +1724,157 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" ht="28.8" spans="1:3">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="3" ht="43.2" spans="1:3">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1"/>
-    <row r="5" ht="14.25" customHeight="1" spans="1:3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
         <v>28</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>29</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1"/>
-    <row r="7" ht="14.25" customHeight="1" spans="1:3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
         <v>31</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>32</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1" spans="1:3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>35</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" ht="14.25" customHeight="1" spans="1:3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
         <v>37</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>38</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" ht="14.25" customHeight="1" spans="1:3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
         <v>40</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>41</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" ht="14.25" customHeight="1" spans="1:3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
         <v>43</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" ht="14.25" customHeight="1" spans="1:3">
-      <c r="A12" t="s">
+    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
         <v>46</v>
-      </c>
-      <c r="B12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1" spans="1:3">
-      <c r="A14" t="s">
-        <v>49</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="15" ht="14.25" customHeight="1" spans="1:3">
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
-    <row r="16" ht="14.25" customHeight="1"/>
-    <row r="17" ht="28.8" spans="1:3">
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -3446,39 +2833,35 @@
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4444444444444" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.8888888888889" customWidth="1"/>
-    <col min="2" max="2" width="30.1111111111111" customWidth="1"/>
-    <col min="3" max="3" width="60.3333333333333" customWidth="1"/>
-    <col min="4" max="26" width="65.4444444444444" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1" spans="1:26">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -3503,21 +2886,21 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1"/>
-    <row r="3" ht="14.25" customHeight="1"/>
-    <row r="4" ht="14.25" customHeight="1"/>
-    <row r="5" ht="14.25" customHeight="1"/>
-    <row r="6" ht="14.25" customHeight="1"/>
-    <row r="7" ht="14.25" customHeight="1"/>
-    <row r="8" ht="14.25" customHeight="1"/>
-    <row r="9" ht="14.25" customHeight="1"/>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -4504,6 +3887,5 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>